<commit_message>
Use zero indexed city ids
</commit_message>
<xml_diff>
--- a/project5/Cost.xlsx
+++ b/project5/Cost.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NUC\Desktop\TSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iver\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,8 +32,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +52,13 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -76,10 +83,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,172 +370,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="D1" s="3">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="E1" s="3">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="F1" s="3">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="G1" s="3">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="H1" s="3">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="I1" s="3">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
+      <c r="J1" s="3">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
+      <c r="K1" s="3">
         <v>9</v>
       </c>
-      <c r="K1" s="1">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1">
+      <c r="L1" s="3">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3">
         <v>11</v>
       </c>
-      <c r="M1" s="1">
+      <c r="N1" s="3">
         <v>12</v>
       </c>
-      <c r="N1" s="1">
+      <c r="O1" s="3">
         <v>13</v>
       </c>
-      <c r="O1" s="1">
+      <c r="P1" s="3">
         <v>14</v>
       </c>
-      <c r="P1" s="1">
+      <c r="Q1" s="3">
         <v>15</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="R1" s="3">
         <v>16</v>
       </c>
-      <c r="R1" s="1">
+      <c r="S1" s="3">
         <v>17</v>
       </c>
-      <c r="S1" s="1">
+      <c r="T1" s="3">
         <v>18</v>
       </c>
-      <c r="T1" s="1">
+      <c r="U1" s="3">
         <v>19</v>
       </c>
-      <c r="U1" s="1">
+      <c r="V1" s="3">
         <v>20</v>
       </c>
-      <c r="V1" s="1">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1">
+      <c r="W1" s="3">
+        <v>21</v>
+      </c>
+      <c r="X1" s="3">
         <v>22</v>
       </c>
-      <c r="X1" s="1">
+      <c r="Y1" s="3">
         <v>23</v>
       </c>
-      <c r="Y1" s="1">
+      <c r="Z1" s="3">
         <v>24</v>
       </c>
-      <c r="Z1" s="1">
+      <c r="AA1" s="3">
         <v>25</v>
       </c>
-      <c r="AA1" s="1">
+      <c r="AB1" s="3">
         <v>26</v>
       </c>
-      <c r="AB1" s="1">
+      <c r="AC1" s="3">
         <v>27</v>
       </c>
-      <c r="AC1" s="1">
+      <c r="AD1" s="3">
         <v>28</v>
       </c>
-      <c r="AD1" s="1">
+      <c r="AE1" s="3">
         <v>29</v>
       </c>
-      <c r="AE1" s="1">
+      <c r="AF1" s="3">
         <v>30</v>
       </c>
-      <c r="AF1" s="1">
+      <c r="AG1" s="3">
         <v>31</v>
       </c>
-      <c r="AG1" s="1">
+      <c r="AH1" s="3">
         <v>32</v>
       </c>
-      <c r="AH1" s="1">
+      <c r="AI1" s="3">
         <v>33</v>
       </c>
-      <c r="AI1" s="1">
-        <v>34</v>
-      </c>
-      <c r="AJ1" s="1">
+      <c r="AJ1" s="3">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="3">
         <v>35</v>
       </c>
-      <c r="AK1" s="1">
+      <c r="AL1" s="3">
         <v>36</v>
       </c>
-      <c r="AL1" s="1">
+      <c r="AM1" s="3">
         <v>37</v>
       </c>
-      <c r="AM1" s="1">
+      <c r="AN1" s="3">
         <v>38</v>
       </c>
-      <c r="AN1" s="1">
+      <c r="AO1" s="3">
         <v>39</v>
       </c>
-      <c r="AO1" s="1">
+      <c r="AP1" s="3">
         <v>40</v>
       </c>
-      <c r="AP1" s="1">
+      <c r="AQ1" s="3">
         <v>41</v>
       </c>
-      <c r="AQ1" s="1">
+      <c r="AR1" s="3">
         <v>42</v>
       </c>
-      <c r="AR1" s="1">
+      <c r="AS1" s="3">
         <v>43</v>
       </c>
-      <c r="AS1" s="1">
+      <c r="AT1" s="3">
         <v>44</v>
       </c>
-      <c r="AT1" s="1">
+      <c r="AU1" s="3">
         <v>45</v>
       </c>
-      <c r="AU1" s="1">
+      <c r="AV1" s="3">
         <v>46</v>
       </c>
-      <c r="AV1" s="1">
+      <c r="AW1" s="3">
         <v>47</v>
       </c>
-      <c r="AW1" s="1">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    </row>
+    <row r="2" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -536,9 +542,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
+    <row r="4" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -550,9 +556,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>4</v>
+    <row r="5" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>8</v>
@@ -567,9 +573,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>5</v>
+    <row r="6" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>4</v>
       </c>
       <c r="B6">
         <v>21</v>
@@ -587,9 +593,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>6</v>
+    <row r="7" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -610,9 +616,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>7</v>
+    <row r="8" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>6</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -636,9 +642,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>8</v>
+    <row r="9" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>7</v>
       </c>
       <c r="B9">
         <v>5</v>
@@ -665,9 +671,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>9</v>
+    <row r="10" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
       </c>
       <c r="B10">
         <v>98</v>
@@ -697,9 +703,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>10</v>
+    <row r="11" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>9</v>
       </c>
       <c r="B11">
         <v>5</v>
@@ -732,9 +738,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>11</v>
+    <row r="12" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>10</v>
       </c>
       <c r="B12">
         <v>2</v>
@@ -770,9 +776,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>12</v>
+    <row r="13" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>11</v>
       </c>
       <c r="B13">
         <v>25</v>
@@ -811,9 +817,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
+    <row r="14" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>12</v>
       </c>
       <c r="B14">
         <v>19</v>
@@ -855,9 +861,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>14</v>
+    <row r="15" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>13</v>
       </c>
       <c r="B15">
         <v>21</v>
@@ -902,9 +908,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
+    <row r="16" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>14</v>
       </c>
       <c r="B16">
         <v>2</v>
@@ -952,9 +958,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>16</v>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>15</v>
       </c>
       <c r="B17">
         <v>14</v>
@@ -1005,9 +1011,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>17</v>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>16</v>
       </c>
       <c r="B18">
         <v>38</v>
@@ -1061,9 +1067,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>18</v>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>17</v>
       </c>
       <c r="B19">
         <v>26</v>
@@ -1120,9 +1126,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>19</v>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>18</v>
       </c>
       <c r="B20">
         <v>33</v>
@@ -1182,9 +1188,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>20</v>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>19</v>
       </c>
       <c r="B21">
         <v>36</v>
@@ -1247,9 +1253,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>21</v>
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -1315,9 +1321,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>22</v>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>21</v>
       </c>
       <c r="B23">
         <v>10</v>
@@ -1386,9 +1392,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>23</v>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>22</v>
       </c>
       <c r="B24">
         <v>9</v>
@@ -1460,9 +1466,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>24</v>
+    <row r="25" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>23</v>
       </c>
       <c r="B25">
         <v>10</v>
@@ -1537,9 +1543,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>25</v>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>24</v>
       </c>
       <c r="B26">
         <v>2</v>
@@ -1617,9 +1623,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>26</v>
+    <row r="27" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>25</v>
       </c>
       <c r="B27">
         <v>19</v>
@@ -1700,9 +1706,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>27</v>
+    <row r="28" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>26</v>
       </c>
       <c r="B28">
         <v>11</v>
@@ -1786,9 +1792,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
-        <v>28</v>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>27</v>
       </c>
       <c r="B29">
         <v>12</v>
@@ -1875,9 +1881,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>29</v>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>28</v>
       </c>
       <c r="B30">
         <v>35</v>
@@ -1967,9 +1973,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>30</v>
+    <row r="31" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>29</v>
       </c>
       <c r="B31">
         <v>31</v>
@@ -2062,9 +2068,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>31</v>
+    <row r="32" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>30</v>
       </c>
       <c r="B32">
         <v>56</v>
@@ -2160,9 +2166,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
-        <v>32</v>
+    <row r="33" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>31</v>
       </c>
       <c r="B33">
         <v>21</v>
@@ -2261,9 +2267,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>33</v>
+    <row r="34" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>32</v>
       </c>
       <c r="B34">
         <v>41</v>
@@ -2365,9 +2371,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>34</v>
+    <row r="35" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>33</v>
       </c>
       <c r="B35">
         <v>11</v>
@@ -2472,9 +2478,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <v>35</v>
+    <row r="36" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>34</v>
       </c>
       <c r="B36">
         <v>75</v>
@@ -2582,9 +2588,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <v>36</v>
+    <row r="37" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>35</v>
       </c>
       <c r="B37">
         <v>41</v>
@@ -2695,9 +2701,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <v>37</v>
+    <row r="38" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>36</v>
       </c>
       <c r="B38">
         <v>2</v>
@@ -2811,9 +2817,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>38</v>
+    <row r="39" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>37</v>
       </c>
       <c r="B39">
         <v>24</v>
@@ -2930,9 +2936,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
-        <v>39</v>
+    <row r="40" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>38</v>
       </c>
       <c r="B40">
         <v>13</v>
@@ -3052,9 +3058,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
-        <v>40</v>
+    <row r="41" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>39</v>
       </c>
       <c r="B41">
         <v>10</v>
@@ -3177,9 +3183,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
-        <v>41</v>
+    <row r="42" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A42" s="3">
+        <v>40</v>
       </c>
       <c r="B42">
         <v>71</v>
@@ -3305,9 +3311,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>42</v>
+    <row r="43" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A43" s="3">
+        <v>41</v>
       </c>
       <c r="B43">
         <v>48</v>
@@ -3436,9 +3442,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>43</v>
+    <row r="44" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A44" s="3">
+        <v>42</v>
       </c>
       <c r="B44">
         <v>10</v>
@@ -3570,9 +3576,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>44</v>
+    <row r="45" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A45" s="3">
+        <v>43</v>
       </c>
       <c r="B45">
         <v>21</v>
@@ -3707,9 +3713,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
-        <v>45</v>
+    <row r="46" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A46" s="3">
+        <v>44</v>
       </c>
       <c r="B46">
         <v>11</v>
@@ -3847,9 +3853,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1">
-        <v>46</v>
+    <row r="47" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A47" s="3">
+        <v>45</v>
       </c>
       <c r="B47">
         <v>5</v>
@@ -3990,9 +3996,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>47</v>
+    <row r="48" spans="1:48" x14ac:dyDescent="0.3">
+      <c r="A48" s="3">
+        <v>46</v>
       </c>
       <c r="B48">
         <v>12</v>
@@ -4136,9 +4142,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:49" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>48</v>
+    <row r="49" spans="1:49" x14ac:dyDescent="0.3">
+      <c r="A49" s="3">
+        <v>47</v>
       </c>
       <c r="B49">
         <v>14</v>
@@ -4285,85 +4291,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:49" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
     </row>
   </sheetData>

</xml_diff>